<commit_message>
add excel file change
</commit_message>
<xml_diff>
--- a/ManualRun.xlsx
+++ b/ManualRun.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\2ND DEGREE\12. Data structure and algorithm\Project\project_datastr_and_algrm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0236096-52A8-463B-AE4E-E214EBD99D15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F146C5-C97C-43BA-920C-4816CB2FCA18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="675" yWindow="2805" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{DF248374-21CA-4876-98EF-42F10EA42DAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="25">
   <si>
     <t>1</t>
   </si>
@@ -101,6 +102,18 @@
   <si>
     <t>phải đúng thứ tự để tránh ngược dấu, nhất là phép - và phép /</t>
   </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
 </sst>
 </file>
 
@@ -141,7 +154,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -334,11 +347,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -426,6 +452,93 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1282,8 +1395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28C4773C-6C08-4F30-9CE3-2934D7AE2E79}">
   <dimension ref="A1:U37"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="Q31" sqref="Q31"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2259,11 +2372,788 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BEF833B-7543-4CAD-95DD-82CDF07BCE85}">
+  <dimension ref="A1:U33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="37"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="30"/>
+      <c r="B1" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="31"/>
+      <c r="U1" s="32"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="33"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="36"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="38"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
+      <c r="Q3" s="39"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="40"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="42"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="41"/>
+      <c r="L4" s="41"/>
+      <c r="M4" s="41"/>
+      <c r="N4" s="41"/>
+      <c r="O4" s="41"/>
+      <c r="P4" s="41"/>
+      <c r="Q4" s="41"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="40"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="41"/>
+      <c r="J5" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" s="41"/>
+      <c r="M5" s="41"/>
+      <c r="N5" s="41"/>
+      <c r="O5" s="41"/>
+      <c r="P5" s="41"/>
+      <c r="Q5" s="41"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="40"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="J6" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="K6" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="L6" s="41" t="s">
+        <v>2</v>
+      </c>
+      <c r="M6" s="41" t="s">
+        <v>2</v>
+      </c>
+      <c r="N6" s="41"/>
+      <c r="O6" s="41"/>
+      <c r="P6" s="41"/>
+      <c r="Q6" s="41"/>
+    </row>
+    <row r="7" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="I7" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="L7" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="M7" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="N7" s="44"/>
+      <c r="O7" s="44"/>
+      <c r="P7" s="44"/>
+      <c r="Q7" s="44"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="45"/>
+      <c r="B8" s="46"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="46"/>
+      <c r="L8" s="46"/>
+      <c r="M8" s="46"/>
+      <c r="N8" s="46"/>
+      <c r="O8" s="46"/>
+      <c r="P8" s="47"/>
+      <c r="Q8" s="48"/>
+      <c r="R8" s="48"/>
+      <c r="S8" s="48"/>
+      <c r="T8" s="48"/>
+      <c r="U8" s="48"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="49"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="50"/>
+      <c r="I9" s="50"/>
+      <c r="J9" s="50"/>
+      <c r="K9" s="50"/>
+      <c r="L9" s="50"/>
+      <c r="M9" s="50"/>
+      <c r="N9" s="50"/>
+      <c r="O9" s="50"/>
+      <c r="P9" s="51"/>
+      <c r="Q9" s="51"/>
+      <c r="R9" s="51"/>
+      <c r="S9" s="51"/>
+      <c r="T9" s="51"/>
+      <c r="U9" s="51"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="49"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="50"/>
+      <c r="H10" s="50"/>
+      <c r="I10" s="50"/>
+      <c r="J10" s="50"/>
+      <c r="K10" s="50"/>
+      <c r="L10" s="50"/>
+      <c r="M10" s="50"/>
+      <c r="N10" s="50"/>
+      <c r="O10" s="50"/>
+      <c r="P10" s="51"/>
+      <c r="Q10" s="51"/>
+      <c r="R10" s="51"/>
+      <c r="S10" s="51"/>
+      <c r="T10" s="51"/>
+      <c r="U10" s="51"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="49"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="50"/>
+      <c r="I11" s="50"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="50"/>
+      <c r="L11" s="50"/>
+      <c r="M11" s="50"/>
+      <c r="N11" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="O11" s="50"/>
+      <c r="P11" s="51"/>
+      <c r="Q11" s="51"/>
+      <c r="R11" s="51"/>
+      <c r="S11" s="51"/>
+      <c r="T11" s="51"/>
+      <c r="U11" s="51"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="49"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
+      <c r="H12" s="50"/>
+      <c r="I12" s="50"/>
+      <c r="J12" s="50"/>
+      <c r="K12" s="50"/>
+      <c r="L12" s="50"/>
+      <c r="M12" s="50"/>
+      <c r="N12" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="O12" s="50"/>
+      <c r="P12" s="51"/>
+      <c r="Q12" s="51"/>
+      <c r="R12" s="51"/>
+      <c r="S12" s="51"/>
+      <c r="T12" s="51"/>
+      <c r="U12" s="51"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="49"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="53"/>
+      <c r="J13" s="53"/>
+      <c r="K13" s="53"/>
+      <c r="L13" s="53"/>
+      <c r="M13" s="53">
+        <v>6</v>
+      </c>
+      <c r="N13" s="53">
+        <v>6</v>
+      </c>
+      <c r="O13" s="50"/>
+      <c r="P13" s="50"/>
+      <c r="Q13" s="50"/>
+      <c r="R13" s="50"/>
+      <c r="S13" s="50"/>
+      <c r="T13" s="50"/>
+      <c r="U13" s="51"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="52"/>
+      <c r="B14" s="53"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="53"/>
+      <c r="F14" s="53"/>
+      <c r="G14" s="53"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="53"/>
+      <c r="K14" s="53"/>
+      <c r="L14" s="53" t="s">
+        <v>5</v>
+      </c>
+      <c r="M14" s="53" t="s">
+        <v>5</v>
+      </c>
+      <c r="N14" s="53" t="s">
+        <v>5</v>
+      </c>
+      <c r="O14" s="53"/>
+      <c r="P14" s="53"/>
+      <c r="Q14" s="53"/>
+      <c r="R14" s="53"/>
+      <c r="S14" s="53"/>
+      <c r="T14" s="53"/>
+      <c r="U14" s="53"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="52"/>
+      <c r="B15" s="53"/>
+      <c r="C15" s="53"/>
+      <c r="D15" s="53"/>
+      <c r="E15" s="53"/>
+      <c r="F15" s="53"/>
+      <c r="G15" s="53"/>
+      <c r="H15" s="53"/>
+      <c r="I15" s="53"/>
+      <c r="J15" s="53"/>
+      <c r="K15" s="53"/>
+      <c r="L15" s="54" t="s">
+        <v>23</v>
+      </c>
+      <c r="M15" s="54" t="s">
+        <v>23</v>
+      </c>
+      <c r="N15" s="54" t="s">
+        <v>23</v>
+      </c>
+      <c r="O15" s="53"/>
+      <c r="P15" s="53"/>
+      <c r="Q15" s="53"/>
+      <c r="R15" s="53"/>
+      <c r="S15" s="53"/>
+      <c r="T15" s="53"/>
+      <c r="U15" s="53"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="52"/>
+      <c r="B16" s="53"/>
+      <c r="C16" s="53"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="53"/>
+      <c r="G16" s="53"/>
+      <c r="H16" s="53"/>
+      <c r="I16" s="53"/>
+      <c r="J16" s="53"/>
+      <c r="K16" s="53">
+        <v>5</v>
+      </c>
+      <c r="L16" s="53">
+        <v>5</v>
+      </c>
+      <c r="M16" s="53">
+        <v>5</v>
+      </c>
+      <c r="N16" s="53">
+        <v>5</v>
+      </c>
+      <c r="O16" s="53"/>
+      <c r="P16" s="53"/>
+      <c r="Q16" s="53"/>
+      <c r="R16" s="53"/>
+      <c r="S16" s="53"/>
+      <c r="T16" s="53"/>
+      <c r="U16" s="53"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A17" s="52"/>
+      <c r="B17" s="53"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="53"/>
+      <c r="G17" s="53"/>
+      <c r="H17" s="53"/>
+      <c r="I17" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="J17" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="K17" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="L17" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="M17" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="N17" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="O17" s="53"/>
+      <c r="P17" s="53"/>
+      <c r="Q17" s="53"/>
+      <c r="R17" s="53"/>
+      <c r="S17" s="53"/>
+      <c r="T17" s="53"/>
+      <c r="U17" s="53"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A18" s="52"/>
+      <c r="B18" s="53"/>
+      <c r="C18" s="53"/>
+      <c r="D18" s="53"/>
+      <c r="E18" s="53"/>
+      <c r="F18" s="53"/>
+      <c r="G18" s="53"/>
+      <c r="H18" s="53">
+        <v>9</v>
+      </c>
+      <c r="I18" s="53">
+        <v>9</v>
+      </c>
+      <c r="J18" s="53">
+        <v>9</v>
+      </c>
+      <c r="K18" s="53">
+        <v>9</v>
+      </c>
+      <c r="L18" s="53">
+        <v>9</v>
+      </c>
+      <c r="M18" s="53">
+        <v>9</v>
+      </c>
+      <c r="N18" s="53">
+        <v>9</v>
+      </c>
+      <c r="O18" s="53"/>
+      <c r="P18" s="53"/>
+      <c r="Q18" s="53"/>
+      <c r="R18" s="53"/>
+      <c r="S18" s="53"/>
+      <c r="T18" s="53"/>
+      <c r="U18" s="53"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" s="52"/>
+      <c r="B19" s="53"/>
+      <c r="C19" s="53"/>
+      <c r="D19" s="53"/>
+      <c r="E19" s="53"/>
+      <c r="F19" s="53">
+        <v>11</v>
+      </c>
+      <c r="G19" s="53">
+        <v>11</v>
+      </c>
+      <c r="H19" s="53">
+        <v>11</v>
+      </c>
+      <c r="I19" s="53">
+        <v>11</v>
+      </c>
+      <c r="J19" s="53">
+        <v>11</v>
+      </c>
+      <c r="K19" s="53">
+        <v>11</v>
+      </c>
+      <c r="L19" s="53">
+        <v>11</v>
+      </c>
+      <c r="M19" s="53">
+        <v>11</v>
+      </c>
+      <c r="N19" s="53">
+        <v>11</v>
+      </c>
+      <c r="O19" s="53"/>
+      <c r="P19" s="53"/>
+      <c r="Q19" s="53"/>
+      <c r="R19" s="53"/>
+      <c r="S19" s="53"/>
+      <c r="T19" s="53"/>
+      <c r="U19" s="53"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" s="52"/>
+      <c r="B20" s="53"/>
+      <c r="C20" s="53">
+        <v>2</v>
+      </c>
+      <c r="D20" s="53">
+        <v>2</v>
+      </c>
+      <c r="E20" s="53">
+        <v>2</v>
+      </c>
+      <c r="F20" s="53">
+        <v>2</v>
+      </c>
+      <c r="G20" s="53">
+        <v>2</v>
+      </c>
+      <c r="H20" s="53">
+        <v>2</v>
+      </c>
+      <c r="I20" s="53">
+        <v>2</v>
+      </c>
+      <c r="J20" s="53">
+        <v>2</v>
+      </c>
+      <c r="K20" s="53">
+        <v>2</v>
+      </c>
+      <c r="L20" s="53">
+        <v>2</v>
+      </c>
+      <c r="M20" s="53">
+        <v>2</v>
+      </c>
+      <c r="N20" s="53">
+        <v>2</v>
+      </c>
+      <c r="O20" s="53"/>
+      <c r="P20" s="53"/>
+      <c r="Q20" s="53"/>
+      <c r="R20" s="53"/>
+      <c r="S20" s="53"/>
+      <c r="T20" s="53"/>
+      <c r="U20" s="53"/>
+    </row>
+    <row r="21" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="55" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="56">
+        <v>0</v>
+      </c>
+      <c r="C21" s="58">
+        <v>0</v>
+      </c>
+      <c r="D21" s="58">
+        <v>0</v>
+      </c>
+      <c r="E21" s="58">
+        <v>0</v>
+      </c>
+      <c r="F21" s="58">
+        <v>0</v>
+      </c>
+      <c r="G21" s="58">
+        <v>0</v>
+      </c>
+      <c r="H21" s="58">
+        <v>0</v>
+      </c>
+      <c r="I21" s="58">
+        <v>0</v>
+      </c>
+      <c r="J21" s="58">
+        <v>0</v>
+      </c>
+      <c r="K21" s="58">
+        <v>0</v>
+      </c>
+      <c r="L21" s="58">
+        <v>0</v>
+      </c>
+      <c r="M21" s="58">
+        <v>0</v>
+      </c>
+      <c r="N21" s="58">
+        <v>0</v>
+      </c>
+      <c r="O21" s="56"/>
+      <c r="P21" s="56"/>
+      <c r="Q21" s="56"/>
+      <c r="R21" s="56"/>
+      <c r="S21" s="56"/>
+      <c r="T21" s="56"/>
+      <c r="U21" s="56"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B28" s="37">
+        <v>-2</v>
+      </c>
+      <c r="C28" s="37">
+        <v>-11</v>
+      </c>
+      <c r="D28" s="37">
+        <v>9</v>
+      </c>
+      <c r="E28" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="F28" s="37">
+        <v>5</v>
+      </c>
+      <c r="G28" s="57" t="s">
+        <v>23</v>
+      </c>
+      <c r="H28" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="I28" s="37">
+        <v>6.5</v>
+      </c>
+      <c r="J28" s="57" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="D31" s="37">
+        <v>9</v>
+      </c>
+      <c r="F31" s="37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C32" s="37">
+        <v>-11</v>
+      </c>
+      <c r="D32" s="37">
+        <v>-11</v>
+      </c>
+      <c r="E32" s="37">
+        <v>-2</v>
+      </c>
+      <c r="F32" s="37">
+        <v>-2</v>
+      </c>
+      <c r="G32" s="37">
+        <v>-0.4</v>
+      </c>
+      <c r="I32" s="37">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" s="37">
+        <v>-2</v>
+      </c>
+      <c r="C33" s="37">
+        <v>-2</v>
+      </c>
+      <c r="D33" s="37">
+        <v>-2</v>
+      </c>
+      <c r="E33" s="37">
+        <v>-2</v>
+      </c>
+      <c r="F33" s="37">
+        <v>-2</v>
+      </c>
+      <c r="G33" s="37">
+        <v>-2</v>
+      </c>
+      <c r="H33" s="37">
+        <v>0.8</v>
+      </c>
+      <c r="I33" s="37">
+        <v>0.8</v>
+      </c>
+      <c r="J33" s="37">
+        <v>-5.7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43DCEA1D-AD05-495E-99FF-9479D5A6F57C}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>